<commit_message>
performance test case added..
</commit_message>
<xml_diff>
--- a/test_case/authentication/login/login_functional_testing.xlsx
+++ b/test_case/authentication/login/login_functional_testing.xlsx
@@ -1545,82 +1545,82 @@
     </dxf>
   </dxfs>
   <tableStyles count="16">
-    <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{93446441-874B-4248-A3A0-5246079B9B60}">
+    <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{930069FA-E697-4F16-A4C6-487A41955359}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="firstRowStripe" dxfId="8"/>
       <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
-    <tableStyle name="1419-style" pivot="0" count="3" xr9:uid="{71676B1D-E839-4526-A88A-D30C8831C528}">
+    <tableStyle name="1419-style" pivot="0" count="3" xr9:uid="{93DE9B87-C5B9-4688-9EFD-F785908A75E4}">
       <tableStyleElement type="headerRow" dxfId="12"/>
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="2147-style" pivot="0" count="3" xr9:uid="{0E8F339F-1109-4451-93CD-7364C6C4E805}">
+    <tableStyle name="2147-style" pivot="0" count="3" xr9:uid="{5E7387E6-436A-4654-89E9-DE34712F3DD1}">
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
       <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
-    <tableStyle name="2170-style" pivot="0" count="3" xr9:uid="{C0B81567-ED9D-4889-B085-2D7D2DA8B4BF}">
+    <tableStyle name="2170-style" pivot="0" count="3" xr9:uid="{8835248D-A9E6-43F9-ADA6-FD01B7731358}">
       <tableStyleElement type="headerRow" dxfId="18"/>
       <tableStyleElement type="firstRowStripe" dxfId="17"/>
       <tableStyleElement type="secondRowStripe" dxfId="16"/>
     </tableStyle>
-    <tableStyle name="2177-style" pivot="0" count="3" xr9:uid="{F52E82A2-6C5E-4E38-B1D2-F1CB78773C8E}">
+    <tableStyle name="2177-style" pivot="0" count="3" xr9:uid="{978E2D3C-F1A0-4DC3-8ADD-A59B8AFE402C}">
       <tableStyleElement type="headerRow" dxfId="21"/>
       <tableStyleElement type="firstRowStripe" dxfId="20"/>
       <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
-    <tableStyle name="2253-style" pivot="0" count="3" xr9:uid="{95EE6058-5C06-4D10-9DDD-A210BC5A74DB}">
+    <tableStyle name="2253-style" pivot="0" count="3" xr9:uid="{37E695B7-CAF1-4BCD-A1B2-7CBD7AB7C7FE}">
       <tableStyleElement type="headerRow" dxfId="24"/>
       <tableStyleElement type="firstRowStripe" dxfId="23"/>
       <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
-    <tableStyle name="2255-style" pivot="0" count="3" xr9:uid="{71AAC183-E923-448F-AEA2-E8B879730CF0}">
+    <tableStyle name="2255-style" pivot="0" count="3" xr9:uid="{3090E593-EE7B-413B-AD0C-3C268554940D}">
       <tableStyleElement type="headerRow" dxfId="27"/>
       <tableStyleElement type="firstRowStripe" dxfId="26"/>
       <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
-    <tableStyle name="2274-style" pivot="0" count="3" xr9:uid="{EB4BCB03-3FC7-4289-A93F-4BA6925579AF}">
+    <tableStyle name="2274-style" pivot="0" count="3" xr9:uid="{8159CFEA-B488-4BBC-8F44-97A8235911A7}">
       <tableStyleElement type="headerRow" dxfId="30"/>
       <tableStyleElement type="firstRowStripe" dxfId="29"/>
       <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
-    <tableStyle name="2277-style" pivot="0" count="3" xr9:uid="{8580C86D-325D-4AB5-980A-6991AAA55E84}">
+    <tableStyle name="2277-style" pivot="0" count="3" xr9:uid="{6326D451-0524-4402-A870-14BBE6A3B8DD}">
       <tableStyleElement type="headerRow" dxfId="33"/>
       <tableStyleElement type="firstRowStripe" dxfId="32"/>
       <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
-    <tableStyle name="2279-style" pivot="0" count="3" xr9:uid="{EDE48703-E969-4CF3-BEBE-782D892A6B11}">
+    <tableStyle name="2279-style" pivot="0" count="3" xr9:uid="{E5B7C3C9-556E-476F-B1BF-4D43918C8D31}">
       <tableStyleElement type="headerRow" dxfId="36"/>
       <tableStyleElement type="firstRowStripe" dxfId="35"/>
       <tableStyleElement type="secondRowStripe" dxfId="34"/>
     </tableStyle>
-    <tableStyle name="2280-style" pivot="0" count="3" xr9:uid="{C11A5B3B-64D1-4F74-B6BA-B3C1AB305F04}">
+    <tableStyle name="2280-style" pivot="0" count="3" xr9:uid="{1C85A648-663E-4C6B-AAB9-729028112B8A}">
       <tableStyleElement type="headerRow" dxfId="39"/>
       <tableStyleElement type="firstRowStripe" dxfId="38"/>
       <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
-    <tableStyle name="2283-style" pivot="0" count="3" xr9:uid="{88233A84-F45F-4EC7-B72C-448702D8A11B}">
+    <tableStyle name="2283-style" pivot="0" count="3" xr9:uid="{6B2A9CC8-8056-405D-B030-5DB03572859D}">
       <tableStyleElement type="headerRow" dxfId="42"/>
       <tableStyleElement type="firstRowStripe" dxfId="41"/>
       <tableStyleElement type="secondRowStripe" dxfId="40"/>
     </tableStyle>
-    <tableStyle name="2285-style" pivot="0" count="3" xr9:uid="{7C5BB075-0BF5-453E-9A76-14203F00CC9A}">
+    <tableStyle name="2285-style" pivot="0" count="3" xr9:uid="{BB8AD679-0027-47BF-B286-8BAF40D9122D}">
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
       <tableStyleElement type="secondRowStripe" dxfId="43"/>
     </tableStyle>
-    <tableStyle name="2287-style" pivot="0" count="3" xr9:uid="{D53D1C9D-0101-4138-8585-6945B37A5A38}">
+    <tableStyle name="2287-style" pivot="0" count="3" xr9:uid="{6A04C718-83D7-425D-8924-A41F2E920BCE}">
       <tableStyleElement type="headerRow" dxfId="48"/>
       <tableStyleElement type="firstRowStripe" dxfId="47"/>
       <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="2292-style" pivot="0" count="3" xr9:uid="{20FC19A4-25A8-4EA6-9422-7A56D513FE0C}">
+    <tableStyle name="2292-style" pivot="0" count="3" xr9:uid="{56CBE979-4981-4643-91D9-862C93A89246}">
       <tableStyleElement type="headerRow" dxfId="51"/>
       <tableStyleElement type="firstRowStripe" dxfId="50"/>
       <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
-    <tableStyle name="2293-style" pivot="0" count="3" xr9:uid="{3194AE68-83EF-4D33-AE0E-7CF6072F99AF}">
+    <tableStyle name="2293-style" pivot="0" count="3" xr9:uid="{8800FB9E-A967-4F60-9C29-9432091A4098}">
       <tableStyleElement type="headerRow" dxfId="54"/>
       <tableStyleElement type="firstRowStripe" dxfId="53"/>
       <tableStyleElement type="secondRowStripe" dxfId="52"/>
@@ -1852,9 +1852,9 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4444444444444" defaultRowHeight="15" customHeight="1"/>
@@ -29715,7 +29715,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F13 F4:F12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F13">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>